<commit_message>
gerando os novos xlsx
</commit_message>
<xml_diff>
--- a/Exercicio2/primos_results_10e3.xlsx
+++ b/Exercicio2/primos_results_10e3.xlsx
@@ -432,16 +432,16 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.000168</v>
+        <v>3.4E-05</v>
       </c>
       <c r="E2">
-        <v>0.000883</v>
+        <v>0.000204</v>
       </c>
       <c r="F2">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.001052</v>
+        <v>0.000239</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -455,16 +455,16 @@
         <v>2</v>
       </c>
       <c r="D3">
+        <v>3.4E-05</v>
+      </c>
+      <c r="E3">
         <v>0.000154</v>
       </c>
-      <c r="E3">
-        <v>0.001188</v>
-      </c>
       <c r="F3">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.001343</v>
+        <v>0.000189</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -478,16 +478,16 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>0.000157</v>
+        <v>3.2E-05</v>
       </c>
       <c r="E4">
-        <v>0.000843</v>
+        <v>0.000154</v>
       </c>
       <c r="F4">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.001</v>
+        <v>0.000187</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -501,16 +501,16 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.000157</v>
+        <v>3.3E-05</v>
       </c>
       <c r="E5">
-        <v>0.000894</v>
+        <v>0.000153</v>
       </c>
       <c r="F5">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.001052</v>
+        <v>0.000186</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -524,16 +524,16 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>0.000157</v>
+        <v>3.1E-05</v>
       </c>
       <c r="E6">
-        <v>0.00078</v>
+        <v>0.000148</v>
       </c>
       <c r="F6">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.000937</v>
+        <v>0.000179</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -547,16 +547,16 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>0.00016</v>
+        <v>3.2E-05</v>
       </c>
       <c r="E7">
-        <v>0.000773</v>
+        <v>0.000156</v>
       </c>
       <c r="F7">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.000934</v>
+        <v>0.000188</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -570,16 +570,16 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>0.000161</v>
+        <v>3.2E-05</v>
       </c>
       <c r="E8">
-        <v>0.000713</v>
+        <v>0.000151</v>
       </c>
       <c r="F8">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.000874</v>
+        <v>0.000183</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -593,16 +593,16 @@
         <v>8</v>
       </c>
       <c r="D9">
+        <v>3.2E-05</v>
+      </c>
+      <c r="E9">
         <v>0.00016</v>
       </c>
-      <c r="E9">
-        <v>0.000757</v>
-      </c>
       <c r="F9">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0.000918</v>
+        <v>0.000192</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -616,16 +616,16 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>0.000157</v>
+        <v>3.3E-05</v>
       </c>
       <c r="E10">
-        <v>0.000749</v>
+        <v>0.000149</v>
       </c>
       <c r="F10">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>0.000907</v>
+        <v>0.000182</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -639,16 +639,16 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>0.00016</v>
+        <v>3.2E-05</v>
       </c>
       <c r="E11">
-        <v>0.000782</v>
+        <v>0.000149</v>
       </c>
       <c r="F11">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0.000942</v>
+        <v>0.000181</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -662,16 +662,16 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0.000241</v>
+        <v>5.2E-05</v>
       </c>
       <c r="E12">
-        <v>0.000925</v>
+        <v>0.000181</v>
       </c>
       <c r="F12">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>0.001167</v>
+        <v>0.000233</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -685,16 +685,16 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>0.000232</v>
+        <v>6.999999999999999E-05</v>
       </c>
       <c r="E13">
-        <v>0.000982</v>
+        <v>0.000166</v>
       </c>
       <c r="F13">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>0.001215</v>
+        <v>0.000236</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -708,16 +708,16 @@
         <v>3</v>
       </c>
       <c r="D14">
-        <v>0.000285</v>
+        <v>5E-05</v>
       </c>
       <c r="E14">
-        <v>0.000826</v>
+        <v>0.00016</v>
       </c>
       <c r="F14">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>0.001112</v>
+        <v>0.00021</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -731,16 +731,16 @@
         <v>4</v>
       </c>
       <c r="D15">
-        <v>0.000235</v>
+        <v>4.9E-05</v>
       </c>
       <c r="E15">
-        <v>0.000896</v>
+        <v>0.000156</v>
       </c>
       <c r="F15">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0.001131</v>
+        <v>0.000206</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -754,16 +754,16 @@
         <v>5</v>
       </c>
       <c r="D16">
-        <v>0.000243</v>
+        <v>4.9E-05</v>
       </c>
       <c r="E16">
-        <v>0.000838</v>
+        <v>0.000179</v>
       </c>
       <c r="F16">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>0.001082</v>
+        <v>0.000228</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -777,16 +777,16 @@
         <v>6</v>
       </c>
       <c r="D17">
-        <v>0.000256</v>
+        <v>4.9E-05</v>
       </c>
       <c r="E17">
-        <v>0.000943</v>
+        <v>0.000169</v>
       </c>
       <c r="F17">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>0.0012</v>
+        <v>0.000218</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -800,16 +800,16 @@
         <v>7</v>
       </c>
       <c r="D18">
-        <v>0.000233</v>
+        <v>5.2E-05</v>
       </c>
       <c r="E18">
-        <v>0.000906</v>
+        <v>0.000164</v>
       </c>
       <c r="F18">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>0.001139</v>
+        <v>0.000216</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -823,16 +823,16 @@
         <v>8</v>
       </c>
       <c r="D19">
-        <v>0.00025</v>
+        <v>4.7E-05</v>
       </c>
       <c r="E19">
-        <v>0.000945</v>
+        <v>0.00018</v>
       </c>
       <c r="F19">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>0.001196</v>
+        <v>0.000227</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -846,16 +846,16 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>0.000264</v>
+        <v>4.6E-05</v>
       </c>
       <c r="E20">
-        <v>0.000923</v>
+        <v>0.000177</v>
       </c>
       <c r="F20">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>0.001188</v>
+        <v>0.000224</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -869,16 +869,16 @@
         <v>10</v>
       </c>
       <c r="D21">
-        <v>0.00027</v>
+        <v>5E-05</v>
       </c>
       <c r="E21">
-        <v>0.000835</v>
+        <v>0.000163</v>
       </c>
       <c r="F21">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>0.001105</v>
+        <v>0.000213</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -892,16 +892,16 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>0.000389</v>
+        <v>7.9E-05</v>
       </c>
       <c r="E22">
-        <v>0.000789</v>
+        <v>0.000134</v>
       </c>
       <c r="F22">
-        <v>1E-06</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>0.001179</v>
+        <v>0.000213</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -915,16 +915,16 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>8.3E-05</v>
+        <v>8.899999999999999E-05</v>
       </c>
       <c r="E23">
-        <v>0.000143</v>
+        <v>0.000123</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0.000226</v>
+        <v>0.000213</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -938,16 +938,16 @@
         <v>3</v>
       </c>
       <c r="D24">
-        <v>8.000000000000001E-05</v>
+        <v>7.7E-05</v>
       </c>
       <c r="E24">
-        <v>0.000153</v>
+        <v>0.000161</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>0.000234</v>
+        <v>0.000238</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -961,16 +961,16 @@
         <v>4</v>
       </c>
       <c r="D25">
-        <v>8.000000000000001E-05</v>
+        <v>7.8E-05</v>
       </c>
       <c r="E25">
-        <v>0.000142</v>
+        <v>0.000139</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0.000222</v>
+        <v>0.000217</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -984,16 +984,16 @@
         <v>5</v>
       </c>
       <c r="D26">
-        <v>8.000000000000001E-05</v>
+        <v>7.9E-05</v>
       </c>
       <c r="E26">
-        <v>0.000141</v>
+        <v>0.000156</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0.000221</v>
+        <v>0.000235</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1007,7 +1007,7 @@
         <v>6</v>
       </c>
       <c r="D27">
-        <v>7.9E-05</v>
+        <v>7.7E-05</v>
       </c>
       <c r="E27">
         <v>0.00016</v>
@@ -1016,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0.000239</v>
+        <v>0.000237</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1030,16 +1030,16 @@
         <v>7</v>
       </c>
       <c r="D28">
-        <v>8.000000000000001E-05</v>
+        <v>7.9E-05</v>
       </c>
       <c r="E28">
-        <v>0.000136</v>
+        <v>0.000146</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0.000216</v>
+        <v>0.000225</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1053,16 +1053,16 @@
         <v>8</v>
       </c>
       <c r="D29">
-        <v>8.2E-05</v>
+        <v>7.6E-05</v>
       </c>
       <c r="E29">
-        <v>0.000138</v>
+        <v>0.00013</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
-        <v>0.000221</v>
+        <v>0.000206</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1076,16 +1076,16 @@
         <v>9</v>
       </c>
       <c r="D30">
-        <v>8.1E-05</v>
+        <v>7.8E-05</v>
       </c>
       <c r="E30">
-        <v>0.000138</v>
+        <v>0.000146</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>0.000219</v>
+        <v>0.000224</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1099,16 +1099,16 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>8.1E-05</v>
+        <v>7.6E-05</v>
       </c>
       <c r="E31">
-        <v>0.000132</v>
+        <v>0.000154</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>0.000213</v>
+        <v>0.00023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>